<commit_message>
Model fixes to elec sector BECF, BPMCCS, BCRbQ
</commit_message>
<xml_diff>
--- a/InputData/indst/BNRbI/BAU Nonfuel Revenue by Industry.xlsx
+++ b/InputData/indst/BNRbI/BAU Nonfuel Revenue by Industry.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-minnesota\InputData\indst\TNRbI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Dropbox (Energy Innovation)\Documents\EPS_Models by Region\RMI\Nevada\NV_model\InputData\indst\BNRbI\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FF6C94E-3113-4F94-9F44-8C5284B163EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2978" yWindow="1103" windowWidth="24758" windowHeight="15578"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -20,7 +21,18 @@
   <definedNames>
     <definedName name="currency_conv">About!$A$65</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -561,7 +573,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -808,15 +820,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="9">
-    <cellStyle name="Body: normal cell" xfId="5"/>
-    <cellStyle name="Font: Calibri, 9pt regular" xfId="7"/>
-    <cellStyle name="Footnotes: top row" xfId="3"/>
-    <cellStyle name="Header: bottom row" xfId="6"/>
+    <cellStyle name="Body: normal cell" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Font: Calibri, 9pt regular" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Footnotes: top row" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Header: bottom row" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2"/>
-    <cellStyle name="Parent row" xfId="4"/>
-    <cellStyle name="Table title" xfId="8"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Parent row" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Table title" xfId="8" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1151,23 +1163,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="64" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1175,267 +1187,267 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
         <v>2019</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10" s="27" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B12" s="2">
         <v>2018</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B17" s="27" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B19" s="2">
         <v>2019</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B24" s="27" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B26" s="2">
         <v>2019</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="24">
         <f>1.07*10^9</f>
         <v>1070000000.0000001</v>
@@ -1444,7 +1456,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>0.93665959530026111</v>
       </c>
@@ -1452,7 +1464,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>0.9143273584567535</v>
       </c>
@@ -1462,16 +1474,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B14" r:id="rId1"/>
-    <hyperlink ref="B21" r:id="rId2"/>
-    <hyperlink ref="B28" r:id="rId3"/>
+    <hyperlink ref="B14" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B21" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B28" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AK65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1481,15 +1493,15 @@
       <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.796875" style="21" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="45.6640625" style="21" customWidth="1"/>
-    <col min="3" max="3" width="9.1328125" style="21" customWidth="1"/>
-    <col min="4" max="16384" width="9.1328125" style="21"/>
+    <col min="1" max="1" width="20.85546875" style="21" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="45.7109375" style="21" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="21" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="13" t="s">
         <v>54</v>
       </c>
@@ -1596,8 +1608,8 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:37" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:37" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C3" s="15" t="s">
         <v>55</v>
       </c>
@@ -1608,7 +1620,7 @@
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
     </row>
-    <row r="4" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C4" s="15" t="s">
         <v>56</v>
       </c>
@@ -1621,7 +1633,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C5" s="15" t="s">
         <v>59</v>
       </c>
@@ -1632,7 +1644,7 @@
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
     </row>
-    <row r="6" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C6" s="15" t="s">
         <v>61</v>
       </c>
@@ -1643,7 +1655,7 @@
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
     </row>
-    <row r="10" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
         <v>63</v>
       </c>
@@ -1651,10 +1663,10 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="13"/>
     </row>
-    <row r="12" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="13"/>
       <c r="C12" s="12"/>
       <c r="D12" s="12"/>
@@ -1694,7 +1706,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B13" s="11" t="s">
         <v>66</v>
       </c>
@@ -1804,8 +1816,8 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="14" spans="1:37" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:37" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="17" t="s">
         <v>67</v>
       </c>
@@ -1918,7 +1930,7 @@
         <v>1.8898000000000002E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="17" t="s">
         <v>69</v>
       </c>
@@ -2031,17 +2043,17 @@
         <v>5.8120000000000003E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="7" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="7" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="22" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="17" t="s">
         <v>73</v>
       </c>
@@ -2154,7 +2166,7 @@
         <v>1.1761000000000001E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
         <v>75</v>
       </c>
@@ -2267,7 +2279,7 @@
         <v>1.107E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
         <v>77</v>
       </c>
@@ -2380,12 +2392,12 @@
         <v>1.4662E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="7" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="27" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="17" t="s">
         <v>80</v>
       </c>
@@ -2498,7 +2510,7 @@
         <v>1.7756000000000001E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="17" t="s">
         <v>82</v>
       </c>
@@ -2611,7 +2623,7 @@
         <v>6.1960000000000001E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
         <v>84</v>
       </c>
@@ -2724,7 +2736,7 @@
         <v>-1.7729999999999999E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="17" t="s">
         <v>86</v>
       </c>
@@ -2837,7 +2849,7 @@
         <v>1.0227999999999999E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="17" t="s">
         <v>88</v>
       </c>
@@ -2950,7 +2962,7 @@
         <v>1.4657999999999999E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="17" t="s">
         <v>90</v>
       </c>
@@ -3063,7 +3075,7 @@
         <v>9.9909999999999999E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="17" t="s">
         <v>92</v>
       </c>
@@ -3176,7 +3188,7 @@
         <v>1.7110000000000001E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="17" t="s">
         <v>94</v>
       </c>
@@ -3289,7 +3301,7 @@
         <v>1.9053E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="17" t="s">
         <v>96</v>
       </c>
@@ -3402,7 +3414,7 @@
         <v>1.5769999999999999E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="17" t="s">
         <v>98</v>
       </c>
@@ -3515,7 +3527,7 @@
         <v>-2.7539999999999999E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="17" t="s">
         <v>100</v>
       </c>
@@ -3628,7 +3640,7 @@
         <v>1.9487000000000001E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="17" t="s">
         <v>102</v>
       </c>
@@ -3741,7 +3753,7 @@
         <v>1.8273000000000001E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="17" t="s">
         <v>104</v>
       </c>
@@ -3854,7 +3866,7 @@
         <v>5.829E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="17" t="s">
         <v>106</v>
       </c>
@@ -3967,7 +3979,7 @@
         <v>2.2030000000000001E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="17" t="s">
         <v>108</v>
       </c>
@@ -4080,7 +4092,7 @@
         <v>-2.575E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="17" t="s">
         <v>110</v>
       </c>
@@ -4193,7 +4205,7 @@
         <v>-2.4510000000000001E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="17" t="s">
         <v>112</v>
       </c>
@@ -4306,7 +4318,7 @@
         <v>-4.176E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="17" t="s">
         <v>114</v>
       </c>
@@ -4419,7 +4431,7 @@
         <v>2.3494999999999999E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="17" t="s">
         <v>116</v>
       </c>
@@ -4532,7 +4544,7 @@
         <v>1.8002000000000001E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="17" t="s">
         <v>118</v>
       </c>
@@ -4645,7 +4657,7 @@
         <v>1.2220999999999999E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="17" t="s">
         <v>120</v>
       </c>
@@ -4758,7 +4770,7 @@
         <v>1.6796999999999999E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="17" t="s">
         <v>122</v>
       </c>
@@ -4871,7 +4883,7 @@
         <v>1.9954E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="17" t="s">
         <v>124</v>
       </c>
@@ -4984,7 +4996,7 @@
         <v>9.5680000000000001E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="17" t="s">
         <v>126</v>
       </c>
@@ -5097,7 +5109,7 @@
         <v>-7.7800000000000005E-4</v>
       </c>
     </row>
-    <row r="51" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="17" t="s">
         <v>128</v>
       </c>
@@ -5210,7 +5222,7 @@
         <v>8.8459999999999997E-3</v>
       </c>
     </row>
-    <row r="52" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="17" t="s">
         <v>130</v>
       </c>
@@ -5323,7 +5335,7 @@
         <v>2.0156E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="17" t="s">
         <v>132</v>
       </c>
@@ -5436,7 +5448,7 @@
         <v>1.8870000000000001E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="17" t="s">
         <v>134</v>
       </c>
@@ -5549,7 +5561,7 @@
         <v>2.6143E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="17" t="s">
         <v>136</v>
       </c>
@@ -5662,7 +5674,7 @@
         <v>2.5361000000000002E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="17" t="s">
         <v>138</v>
       </c>
@@ -5775,7 +5787,7 @@
         <v>2.5756000000000001E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="17" t="s">
         <v>140</v>
       </c>
@@ -5888,7 +5900,7 @@
         <v>2.6575999999999999E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="17" t="s">
         <v>142</v>
       </c>
@@ -6001,7 +6013,7 @@
         <v>2.8815E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="17" t="s">
         <v>144</v>
       </c>
@@ -6114,8 +6126,8 @@
         <v>1.7311E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="62" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="62" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="33" t="s">
         <v>146</v>
       </c>
@@ -6155,17 +6167,17 @@
       <c r="AJ62" s="34"/>
       <c r="AK62" s="34"/>
     </row>
-    <row r="63" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B63" s="4" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="64" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B64" s="4" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="65" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B65" s="4" t="s">
         <v>149</v>
       </c>
@@ -6180,35 +6192,35 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AJ22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
-    <col min="2" max="2" width="14.796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.46484375" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.46484375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
         <v>150</v>
       </c>
       <c r="B1" s="30"/>
       <c r="C1" s="30"/>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>152</v>
       </c>
@@ -6229,7 +6241,7 @@
       </c>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>2017</v>
       </c>
@@ -6243,17 +6255,17 @@
         <v>325084.75799999997</v>
       </c>
       <c r="E5">
-        <v>5572.2439999999997</v>
+        <v>3012.223</v>
       </c>
       <c r="F5">
         <f>B5*(E5/D5)</f>
-        <v>2.9482340971519805</v>
+        <v>1.5937454563772566</v>
       </c>
       <c r="G5" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B6" s="31">
         <f>B5/About!A67</f>
         <v>183.63127956305479</v>
@@ -6263,25 +6275,25 @@
       </c>
       <c r="F6">
         <f>F5/About!A67</f>
-        <v>3.1476046494851495</v>
+        <v>1.7015204503044206</v>
       </c>
       <c r="G6" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8" s="27" t="s">
         <v>160</v>
       </c>
       <c r="B8" s="30"/>
       <c r="C8" s="30"/>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>152</v>
       </c>
@@ -6296,7 +6308,7 @@
       </c>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>2018</v>
       </c>
@@ -6308,13 +6320,13 @@
       </c>
       <c r="F12">
         <f>B12*(E5/D5)</f>
-        <v>1.2341445057845499</v>
+        <v>0.6671492608090841</v>
       </c>
       <c r="G12" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B13" s="31">
         <f>B12/About!A68</f>
         <v>78.746413233795309</v>
@@ -6324,20 +6336,20 @@
       </c>
       <c r="F13">
         <f>F12/About!A67</f>
-        <v>1.3176019462961091</v>
+        <v>0.71226437454603642</v>
       </c>
       <c r="G13" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A15" s="27" t="s">
         <v>163</v>
       </c>
       <c r="B15" s="30"/>
       <c r="C15" s="30"/>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>152</v>
       </c>
@@ -6447,7 +6459,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>164</v>
       </c>
@@ -6455,528 +6467,528 @@
         <v>323015.99200000003</v>
       </c>
       <c r="C17" s="28">
-        <v>5572.2439999999997</v>
+        <v>3012.223</v>
       </c>
       <c r="D17" s="28">
-        <v>5610.5749999999998</v>
+        <v>3056.748</v>
       </c>
       <c r="E17" s="28">
-        <v>5648.9070000000002</v>
+        <v>3101.2719999999999</v>
       </c>
       <c r="F17" s="28">
-        <v>5687.2380000000003</v>
+        <v>3145.797</v>
       </c>
       <c r="G17" s="28">
-        <v>5725.5690000000004</v>
+        <v>3190.3220000000001</v>
       </c>
       <c r="H17" s="28">
-        <v>5763.9009999999998</v>
+        <v>3234.846</v>
       </c>
       <c r="I17" s="28">
-        <v>5802.232</v>
+        <v>3279.3710000000001</v>
       </c>
       <c r="J17" s="28">
-        <v>5840.5630000000001</v>
+        <v>3323.895</v>
       </c>
       <c r="K17" s="28">
-        <v>5878.8940000000002</v>
+        <v>3368.42</v>
       </c>
       <c r="L17" s="28">
-        <v>5917.2260000000006</v>
+        <v>3412.9450000000002</v>
       </c>
       <c r="M17" s="28">
-        <v>5955.5569999999998</v>
+        <v>3457.4690000000001</v>
       </c>
       <c r="N17" s="28">
-        <v>5993.8879999999999</v>
+        <v>3501.9940000000001</v>
       </c>
       <c r="O17" s="28">
-        <v>6032.22</v>
+        <v>3546.518</v>
       </c>
       <c r="P17" s="28">
-        <v>6070.5510000000004</v>
+        <v>3591.0430000000001</v>
       </c>
       <c r="Q17" s="28">
-        <v>6108.8820000000014</v>
+        <v>3635.5680000000002</v>
       </c>
       <c r="R17" s="28">
-        <v>6147.2139999999999</v>
+        <v>3680.0920000000001</v>
       </c>
       <c r="S17" s="28">
-        <v>6185.5450000000001</v>
+        <v>3724.6170000000002</v>
       </c>
       <c r="T17" s="28">
-        <v>6223.8760000000002</v>
+        <v>3769.1410000000001</v>
       </c>
       <c r="U17" s="28">
-        <v>6262.2080000000014</v>
+        <v>3813.6660000000002</v>
       </c>
       <c r="V17" s="28">
-        <v>6300.5389999999998</v>
+        <v>3858.1909999999998</v>
       </c>
       <c r="W17" s="28">
-        <v>6338.87</v>
+        <v>3902.7150000000001</v>
       </c>
       <c r="X17" s="28">
-        <v>6377.201</v>
+        <v>3947.24</v>
       </c>
       <c r="Y17" s="28">
-        <v>6415.5330000000004</v>
+        <v>3991.7640000000001</v>
       </c>
       <c r="Z17" s="28">
-        <v>6453.8639999999996</v>
+        <v>4036.2890000000002</v>
       </c>
       <c r="AA17" s="28">
-        <v>6492.1949999999997</v>
+        <v>4080.8139999999999</v>
       </c>
       <c r="AB17" s="28">
-        <v>6530.527</v>
+        <v>4125.3379999999997</v>
       </c>
       <c r="AC17" s="28">
-        <v>6568.8580000000002</v>
+        <v>4169.8630000000003</v>
       </c>
       <c r="AD17" s="28">
-        <v>6607.1890000000003</v>
+        <v>4214.3869999999997</v>
       </c>
       <c r="AE17" s="28">
-        <v>6645.52</v>
+        <v>4258.9120000000003</v>
       </c>
       <c r="AF17" s="28">
-        <v>6683.8519999999999</v>
+        <v>4303.4369999999999</v>
       </c>
       <c r="AG17" s="28">
-        <v>6722.183</v>
+        <v>4347.9610000000002</v>
       </c>
       <c r="AH17" s="28">
-        <v>6760.5140000000001</v>
+        <v>4392.4859999999999</v>
       </c>
       <c r="AI17" s="28">
-        <v>6798.8459999999995</v>
+        <v>4437.01</v>
       </c>
       <c r="AJ17" s="28">
-        <v>6837.1770000000006</v>
-      </c>
-    </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.45">
+        <v>4481.5349999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A19" s="27" t="s">
         <v>165</v>
       </c>
       <c r="B19" s="30"/>
       <c r="C19" s="30"/>
     </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>150</v>
       </c>
       <c r="C20" s="32">
         <f>F6</f>
-        <v>3.1476046494851495</v>
+        <v>1.7015204503044206</v>
       </c>
       <c r="D20" s="29">
         <f t="shared" ref="D20:AJ20" si="0">$C20*(D17/$C17)</f>
-        <v>3.1692567583697238</v>
+        <v>1.726671376397809</v>
       </c>
       <c r="E20" s="29">
         <f t="shared" si="0"/>
-        <v>3.1909094321263045</v>
+        <v>1.7518217376191907</v>
       </c>
       <c r="F20" s="29">
         <f t="shared" si="0"/>
-        <v>3.2125615410108792</v>
+        <v>1.7769726637125787</v>
       </c>
       <c r="G20" s="29">
         <f t="shared" si="0"/>
-        <v>3.2342136498954535</v>
+        <v>1.8021235898059671</v>
       </c>
       <c r="H20" s="29">
         <f t="shared" si="0"/>
-        <v>3.2558663236520338</v>
+        <v>1.8272739510273488</v>
       </c>
       <c r="I20" s="29">
         <f t="shared" si="0"/>
-        <v>3.2775184325366076</v>
+        <v>1.8524248771207372</v>
       </c>
       <c r="J20" s="29">
         <f t="shared" si="0"/>
-        <v>3.2991705414211827</v>
+        <v>1.8775752383421189</v>
       </c>
       <c r="K20" s="29">
         <f t="shared" si="0"/>
-        <v>3.3208226503057565</v>
+        <v>1.9027261644355069</v>
       </c>
       <c r="L20" s="29">
         <f t="shared" si="0"/>
-        <v>3.3424753240623377</v>
+        <v>1.9278770905288953</v>
       </c>
       <c r="M20" s="29">
         <f t="shared" si="0"/>
-        <v>3.3641274329469115</v>
+        <v>1.953027451750277</v>
       </c>
       <c r="N20" s="29">
         <f t="shared" si="0"/>
-        <v>3.3857795418314858</v>
+        <v>1.9781783778436655</v>
       </c>
       <c r="O20" s="29">
         <f t="shared" si="0"/>
-        <v>3.4074322155880665</v>
+        <v>2.0033287390650472</v>
       </c>
       <c r="P20" s="29">
         <f t="shared" si="0"/>
-        <v>3.4290843244726408</v>
+        <v>2.0284796651584354</v>
       </c>
       <c r="Q20" s="29">
         <f t="shared" si="0"/>
-        <v>3.4507364333572155</v>
+        <v>2.0536305912518236</v>
       </c>
       <c r="R20" s="29">
         <f t="shared" si="0"/>
-        <v>3.4723891071137958</v>
+        <v>2.0787809524732053</v>
       </c>
       <c r="S20" s="29">
         <f t="shared" si="0"/>
-        <v>3.49404121599837</v>
+        <v>2.1039318785665935</v>
       </c>
       <c r="T20" s="29">
         <f t="shared" si="0"/>
-        <v>3.5156933248829438</v>
+        <v>2.1290822397879752</v>
       </c>
       <c r="U20" s="29">
         <f t="shared" si="0"/>
-        <v>3.5373459986395259</v>
+        <v>2.1542331658813638</v>
       </c>
       <c r="V20" s="29">
         <f t="shared" si="0"/>
-        <v>3.5589981075240988</v>
+        <v>2.179384091974752</v>
       </c>
       <c r="W20" s="29">
         <f t="shared" si="0"/>
-        <v>3.5806502164086731</v>
+        <v>2.2045344531961333</v>
       </c>
       <c r="X20" s="29">
         <f t="shared" si="0"/>
-        <v>3.6023023252932473</v>
+        <v>2.2296853792895215</v>
       </c>
       <c r="Y20" s="29">
         <f t="shared" si="0"/>
-        <v>3.6239549990498281</v>
+        <v>2.2548357405109036</v>
       </c>
       <c r="Z20" s="29">
         <f t="shared" si="0"/>
-        <v>3.6456071079344023</v>
+        <v>2.2799866666042918</v>
       </c>
       <c r="AA20" s="29">
         <f t="shared" si="0"/>
-        <v>3.6672592168189762</v>
+        <v>2.30513759269768</v>
       </c>
       <c r="AB20" s="29">
         <f t="shared" si="0"/>
-        <v>3.6889118905755574</v>
+        <v>2.3302879539190617</v>
       </c>
       <c r="AC20" s="29">
         <f t="shared" si="0"/>
-        <v>3.7105639994601312</v>
+        <v>2.3554388800124499</v>
       </c>
       <c r="AD20" s="29">
         <f t="shared" si="0"/>
-        <v>3.7322161083447063</v>
+        <v>2.3805892412338316</v>
       </c>
       <c r="AE20" s="29">
         <f t="shared" si="0"/>
-        <v>3.7538682172292801</v>
+        <v>2.4057401673272203</v>
       </c>
       <c r="AF20" s="29">
         <f t="shared" si="0"/>
-        <v>3.7755208909858604</v>
+        <v>2.4308910934206081</v>
       </c>
       <c r="AG20" s="29">
         <f t="shared" si="0"/>
-        <v>3.7971729998704351</v>
+        <v>2.4560414546419902</v>
       </c>
       <c r="AH20" s="29">
         <f t="shared" si="0"/>
-        <v>3.8188251087550094</v>
+        <v>2.4811923807353784</v>
       </c>
       <c r="AI20" s="29">
         <f t="shared" si="0"/>
-        <v>3.8404777825115897</v>
+        <v>2.5063427419567597</v>
       </c>
       <c r="AJ20" s="29">
         <f t="shared" si="0"/>
-        <v>3.8621298913961644</v>
-      </c>
-    </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.45">
+        <v>2.5314936680501479</v>
+      </c>
+    </row>
+    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>166</v>
       </c>
       <c r="D21" s="32">
         <f>F13</f>
-        <v>1.3176019462961091</v>
+        <v>0.71226437454603642</v>
       </c>
       <c r="E21" s="29">
         <f t="shared" ref="E21:AJ21" si="1">$D21*(E17/$D17)</f>
-        <v>1.3266039323323751</v>
+        <v>0.72263907962878704</v>
       </c>
       <c r="F21" s="29">
         <f t="shared" si="1"/>
-        <v>1.3356056835260544</v>
+        <v>0.73301401772530739</v>
       </c>
       <c r="G21" s="29">
         <f t="shared" si="1"/>
-        <v>1.3446074347197332</v>
+        <v>0.74338895582182773</v>
       </c>
       <c r="H21" s="29">
         <f t="shared" si="1"/>
-        <v>1.3536094207559992</v>
+        <v>0.75376366090457825</v>
       </c>
       <c r="I21" s="29">
         <f t="shared" si="1"/>
-        <v>1.3626111719496781</v>
+        <v>0.7641385990010986</v>
       </c>
       <c r="J21" s="29">
         <f t="shared" si="1"/>
-        <v>1.3716129231433574</v>
+        <v>0.77451330408384911</v>
       </c>
       <c r="K21" s="29">
         <f t="shared" si="1"/>
-        <v>1.3806146743370367</v>
+        <v>0.78488824218036946</v>
       </c>
       <c r="L21" s="29">
         <f t="shared" si="1"/>
-        <v>1.3896166603733024</v>
+        <v>0.7952631802768898</v>
       </c>
       <c r="M21" s="29">
         <f t="shared" si="1"/>
-        <v>1.3986184115669813</v>
+        <v>0.80563788535964032</v>
       </c>
       <c r="N21" s="29">
         <f t="shared" si="1"/>
-        <v>1.4076201627606604</v>
+        <v>0.81601282345616066</v>
       </c>
       <c r="O21" s="29">
         <f t="shared" si="1"/>
-        <v>1.4166221487969264</v>
+        <v>0.82638752853891129</v>
       </c>
       <c r="P21" s="29">
         <f t="shared" si="1"/>
-        <v>1.4256238999906057</v>
+        <v>0.83676246663543163</v>
       </c>
       <c r="Q21" s="29">
         <f t="shared" si="1"/>
-        <v>1.434625651184285</v>
+        <v>0.84713740473195198</v>
       </c>
       <c r="R21" s="29">
         <f t="shared" si="1"/>
-        <v>1.4436276372205505</v>
+        <v>0.85751210981470249</v>
       </c>
       <c r="S21" s="29">
         <f t="shared" si="1"/>
-        <v>1.4526293884142294</v>
+        <v>0.86788704791122284</v>
       </c>
       <c r="T21" s="29">
         <f t="shared" si="1"/>
-        <v>1.4616311396079087</v>
+        <v>0.87826175299397347</v>
       </c>
       <c r="U21" s="29">
         <f t="shared" si="1"/>
-        <v>1.4706331256441749</v>
+        <v>0.88863669109049381</v>
       </c>
       <c r="V21" s="29">
         <f t="shared" si="1"/>
-        <v>1.4796348768378536</v>
+        <v>0.89901162918701405</v>
       </c>
       <c r="W21" s="29">
         <f t="shared" si="1"/>
-        <v>1.4886366280315328</v>
+        <v>0.90938633426976456</v>
       </c>
       <c r="X21" s="29">
         <f t="shared" si="1"/>
-        <v>1.4976383792252119</v>
+        <v>0.91976127236628491</v>
       </c>
       <c r="Y21" s="29">
         <f t="shared" si="1"/>
-        <v>1.5066403652614777</v>
+        <v>0.93013597744903553</v>
       </c>
       <c r="Z21" s="29">
         <f t="shared" si="1"/>
-        <v>1.5156421164551568</v>
+        <v>0.94051091554555588</v>
       </c>
       <c r="AA21" s="29">
         <f t="shared" si="1"/>
-        <v>1.5246438676488361</v>
+        <v>0.95088585364207612</v>
       </c>
       <c r="AB21" s="29">
         <f t="shared" si="1"/>
-        <v>1.5336458536851019</v>
+        <v>0.96126055872482663</v>
       </c>
       <c r="AC21" s="29">
         <f t="shared" si="1"/>
-        <v>1.5426476048787809</v>
+        <v>0.9716354968213472</v>
       </c>
       <c r="AD21" s="29">
         <f t="shared" si="1"/>
-        <v>1.5516493560724602</v>
+        <v>0.9820102019040976</v>
       </c>
       <c r="AE21" s="29">
         <f t="shared" si="1"/>
-        <v>1.5606511072661393</v>
+        <v>0.99238514000061806</v>
       </c>
       <c r="AF21" s="29">
         <f t="shared" si="1"/>
-        <v>1.5696530933024051</v>
+        <v>1.0027600780971382</v>
       </c>
       <c r="AG21" s="29">
         <f t="shared" si="1"/>
-        <v>1.5786548444960844</v>
+        <v>1.0131347831798889</v>
       </c>
       <c r="AH21" s="29">
         <f t="shared" si="1"/>
-        <v>1.5876565956897633</v>
+        <v>1.0235097212764093</v>
       </c>
       <c r="AI21" s="29">
         <f t="shared" si="1"/>
-        <v>1.5966585817260293</v>
+        <v>1.0338844263591598</v>
       </c>
       <c r="AJ21" s="29">
         <f t="shared" si="1"/>
-        <v>1.6056603329197086</v>
-      </c>
-    </row>
-    <row r="22" spans="1:36" x14ac:dyDescent="0.45">
+        <v>1.0442593644556801</v>
+      </c>
+    </row>
+    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>167</v>
       </c>
       <c r="D22" s="29">
         <f t="shared" ref="D22:AJ22" si="2">SUM(D20:D21)</f>
-        <v>4.486858704665833</v>
+        <v>2.4389357509438456</v>
       </c>
       <c r="E22" s="29">
         <f t="shared" si="2"/>
-        <v>4.5175133644586793</v>
+        <v>2.4744608172479778</v>
       </c>
       <c r="F22" s="29">
         <f t="shared" si="2"/>
-        <v>4.5481672245369333</v>
+        <v>2.5099866814378862</v>
       </c>
       <c r="G22" s="29">
         <f t="shared" si="2"/>
-        <v>4.5788210846151864</v>
+        <v>2.5455125456277949</v>
       </c>
       <c r="H22" s="29">
         <f t="shared" si="2"/>
-        <v>4.6094757444080328</v>
+        <v>2.5810376119319272</v>
       </c>
       <c r="I22" s="29">
         <f t="shared" si="2"/>
-        <v>4.6401296044862859</v>
+        <v>2.6165634761218359</v>
       </c>
       <c r="J22" s="29">
         <f t="shared" si="2"/>
-        <v>4.6707834645645399</v>
+        <v>2.6520885424259681</v>
       </c>
       <c r="K22" s="29">
         <f t="shared" si="2"/>
-        <v>4.701437324642793</v>
+        <v>2.6876144066158765</v>
       </c>
       <c r="L22" s="29">
         <f t="shared" si="2"/>
-        <v>4.7320919844356402</v>
+        <v>2.7231402708057852</v>
       </c>
       <c r="M22" s="29">
         <f t="shared" si="2"/>
-        <v>4.7627458445138924</v>
+        <v>2.7586653371099175</v>
       </c>
       <c r="N22" s="29">
         <f t="shared" si="2"/>
-        <v>4.7933997045921464</v>
+        <v>2.7941912012998262</v>
       </c>
       <c r="O22" s="29">
         <f t="shared" si="2"/>
-        <v>4.8240543643849927</v>
+        <v>2.8297162676039584</v>
       </c>
       <c r="P22" s="29">
         <f t="shared" si="2"/>
-        <v>4.8547082244632467</v>
+        <v>2.8652421317938668</v>
       </c>
       <c r="Q22" s="29">
         <f t="shared" si="2"/>
-        <v>4.8853620845415007</v>
+        <v>2.9007679959837755</v>
       </c>
       <c r="R22" s="29">
         <f t="shared" si="2"/>
-        <v>4.9160167443343461</v>
+        <v>2.9362930622879078</v>
       </c>
       <c r="S22" s="29">
         <f t="shared" si="2"/>
-        <v>4.9466706044125992</v>
+        <v>2.9718189264778161</v>
       </c>
       <c r="T22" s="29">
         <f t="shared" si="2"/>
-        <v>4.9773244644908523</v>
+        <v>3.0073439927819487</v>
       </c>
       <c r="U22" s="29">
         <f t="shared" si="2"/>
-        <v>5.0079791242837004</v>
+        <v>3.0428698569718575</v>
       </c>
       <c r="V22" s="29">
         <f t="shared" si="2"/>
-        <v>5.0386329843619526</v>
+        <v>3.0783957211617663</v>
       </c>
       <c r="W22" s="29">
         <f t="shared" si="2"/>
-        <v>5.0692868444402057</v>
+        <v>3.1139207874658981</v>
       </c>
       <c r="X22" s="29">
         <f t="shared" si="2"/>
-        <v>5.0999407045184597</v>
+        <v>3.1494466516558064</v>
       </c>
       <c r="Y22" s="29">
         <f t="shared" si="2"/>
-        <v>5.130595364311306</v>
+        <v>3.1849717179599391</v>
       </c>
       <c r="Z22" s="29">
         <f t="shared" si="2"/>
-        <v>5.1612492243895591</v>
+        <v>3.2204975821498478</v>
       </c>
       <c r="AA22" s="29">
         <f t="shared" si="2"/>
-        <v>5.1919030844678122</v>
+        <v>3.2560234463397562</v>
       </c>
       <c r="AB22" s="29">
         <f t="shared" si="2"/>
-        <v>5.2225577442606594</v>
+        <v>3.2915485126438884</v>
       </c>
       <c r="AC22" s="29">
         <f t="shared" si="2"/>
-        <v>5.2532116043389117</v>
+        <v>3.3270743768337971</v>
       </c>
       <c r="AD22" s="29">
         <f t="shared" si="2"/>
-        <v>5.2838654644171665</v>
+        <v>3.3625994431379294</v>
       </c>
       <c r="AE22" s="29">
         <f t="shared" si="2"/>
-        <v>5.3145193244954196</v>
+        <v>3.3981253073278381</v>
       </c>
       <c r="AF22" s="29">
         <f t="shared" si="2"/>
-        <v>5.345173984288266</v>
+        <v>3.433651171517746</v>
       </c>
       <c r="AG22" s="29">
         <f t="shared" si="2"/>
-        <v>5.3758278443665191</v>
+        <v>3.4691762378218791</v>
       </c>
       <c r="AH22" s="29">
         <f t="shared" si="2"/>
-        <v>5.4064817044447722</v>
+        <v>3.5047021020117874</v>
       </c>
       <c r="AI22" s="29">
         <f t="shared" si="2"/>
-        <v>5.4371363642376185</v>
+        <v>3.5402271683159192</v>
       </c>
       <c r="AJ22" s="29">
         <f t="shared" si="2"/>
-        <v>5.4677902243158734</v>
+        <v>3.575753032505828</v>
       </c>
     </row>
   </sheetData>
@@ -6986,23 +6998,23 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:AH11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.46484375" customWidth="1"/>
-    <col min="2" max="2" width="11.46484375" customWidth="1"/>
+    <col min="1" max="1" width="36.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>168</v>
       </c>
@@ -7106,109 +7118,109 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>169</v>
       </c>
       <c r="B2" s="24"/>
       <c r="C2" s="24">
-        <v>372287440.73999989</v>
+        <v>160546239.53999999</v>
       </c>
       <c r="D2" s="24">
-        <v>367683551.91000003</v>
+        <v>158560846.11000001</v>
       </c>
       <c r="E2" s="24">
-        <v>370026067.75999999</v>
+        <v>159571038.96000001</v>
       </c>
       <c r="F2" s="24">
-        <v>378664305.13</v>
+        <v>163296215.72999999</v>
       </c>
       <c r="G2" s="24">
-        <v>386493603.79000002</v>
+        <v>166672543.59</v>
       </c>
       <c r="H2" s="24">
-        <v>393377707.38</v>
+        <v>169641262.97999999</v>
       </c>
       <c r="I2" s="24">
-        <v>400282937.38</v>
+        <v>172619092.97999999</v>
       </c>
       <c r="J2" s="24">
-        <v>406046160.42000002</v>
+        <v>175104440.81999999</v>
       </c>
       <c r="K2" s="24">
-        <v>411826376.99999988</v>
+        <v>177597117</v>
       </c>
       <c r="L2" s="24">
-        <v>418029917.55000001</v>
+        <v>180272348.55000001</v>
       </c>
       <c r="M2" s="24">
-        <v>424248295.3599999</v>
+        <v>182953978.56</v>
       </c>
       <c r="N2" s="24">
-        <v>430537958.75999987</v>
+        <v>185666349.96000001</v>
       </c>
       <c r="O2" s="24">
-        <v>436980435.67000002</v>
+        <v>188444621.06999999</v>
       </c>
       <c r="P2" s="24">
-        <v>443399732.56999999</v>
+        <v>191212895.97</v>
       </c>
       <c r="Q2" s="24">
-        <v>449950665.23000002</v>
+        <v>194037937.83000001</v>
       </c>
       <c r="R2" s="24">
-        <v>457318596.98000002</v>
+        <v>197215304.58000001</v>
       </c>
       <c r="S2" s="24">
-        <v>463549014.01999998</v>
+        <v>199902126.41999999</v>
       </c>
       <c r="T2" s="24">
-        <v>469180010.88999999</v>
+        <v>202330452.69</v>
       </c>
       <c r="U2" s="24">
-        <v>474974012.25999999</v>
+        <v>204829073.46000001</v>
       </c>
       <c r="V2" s="24">
-        <v>480162971.73000002</v>
+        <v>207066774.33000001</v>
       </c>
       <c r="W2" s="24">
-        <v>484235619.91000003</v>
+        <v>208823074.11000001</v>
       </c>
       <c r="X2" s="24">
-        <v>490874010.25999999</v>
+        <v>211685831.46000001</v>
       </c>
       <c r="Y2" s="24">
-        <v>498398297.98000002</v>
+        <v>214930625.58000001</v>
       </c>
       <c r="Z2" s="24">
-        <v>504405309.00999999</v>
+        <v>217521105.21000001</v>
       </c>
       <c r="AA2" s="24">
-        <v>511644634.05999988</v>
+        <v>220643011.25999999</v>
       </c>
       <c r="AB2" s="24">
-        <v>520052816.88999999</v>
+        <v>224268978.69</v>
       </c>
       <c r="AC2" s="24">
-        <v>528860707.29000002</v>
+        <v>228067317.09</v>
       </c>
       <c r="AD2" s="24">
-        <v>537191777.43999994</v>
+        <v>231660030.24000001</v>
       </c>
       <c r="AE2" s="24">
-        <v>545201561.87</v>
+        <v>235114191.27000001</v>
       </c>
       <c r="AF2" s="24">
-        <v>553371783.79999995</v>
+        <v>238637539.80000001</v>
       </c>
       <c r="AG2" s="24">
-        <v>561207525.63</v>
+        <v>242016646.22999999</v>
       </c>
       <c r="AH2" s="24">
-        <v>569084365.13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.45">
+        <v>245413475.72999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>170</v>
       </c>
@@ -7309,211 +7321,211 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>171</v>
       </c>
       <c r="B4" s="24"/>
       <c r="C4" s="24">
-        <v>307007791.19999999</v>
+        <v>0</v>
       </c>
       <c r="D4" s="24">
-        <v>296531171.19999999</v>
+        <v>0</v>
       </c>
       <c r="E4" s="24">
-        <v>280454026.60000002</v>
+        <v>0</v>
       </c>
       <c r="F4" s="24">
-        <v>274225153.39999998</v>
+        <v>0</v>
       </c>
       <c r="G4" s="24">
-        <v>277796644.39999998</v>
+        <v>0</v>
       </c>
       <c r="H4" s="24">
-        <v>280296502.19999999</v>
+        <v>0</v>
       </c>
       <c r="I4" s="24">
-        <v>280172631.19999999</v>
+        <v>0</v>
       </c>
       <c r="J4" s="24">
-        <v>279063835.60000002</v>
+        <v>0</v>
       </c>
       <c r="K4" s="24">
-        <v>277526697.80000001</v>
+        <v>0</v>
       </c>
       <c r="L4" s="24">
-        <v>276175682.19999999</v>
+        <v>0</v>
       </c>
       <c r="M4" s="24">
-        <v>275006595.60000002</v>
+        <v>0</v>
       </c>
       <c r="N4" s="24">
-        <v>273891860</v>
+        <v>0</v>
       </c>
       <c r="O4" s="24">
-        <v>272638968.80000001</v>
+        <v>0</v>
       </c>
       <c r="P4" s="24">
-        <v>273204360</v>
+        <v>0</v>
       </c>
       <c r="Q4" s="24">
-        <v>274067426.60000002</v>
+        <v>0</v>
       </c>
       <c r="R4" s="24">
-        <v>274615882.19999999</v>
+        <v>0</v>
       </c>
       <c r="S4" s="24">
-        <v>275263553.39999998</v>
+        <v>0</v>
       </c>
       <c r="T4" s="24">
-        <v>276112320</v>
+        <v>0</v>
       </c>
       <c r="U4" s="24">
-        <v>277146977.80000001</v>
+        <v>0</v>
       </c>
       <c r="V4" s="24">
-        <v>277895204.39999998</v>
+        <v>0</v>
       </c>
       <c r="W4" s="24">
-        <v>278360944.39999998</v>
+        <v>0</v>
       </c>
       <c r="X4" s="24">
-        <v>279003562.19999999</v>
+        <v>0</v>
       </c>
       <c r="Y4" s="24">
-        <v>278859902.19999999</v>
+        <v>0</v>
       </c>
       <c r="Z4" s="24">
-        <v>278701053.39999998</v>
+        <v>0</v>
       </c>
       <c r="AA4" s="24">
-        <v>278484800</v>
+        <v>0</v>
       </c>
       <c r="AB4" s="24">
-        <v>278062613.39999998</v>
+        <v>0</v>
       </c>
       <c r="AC4" s="24">
-        <v>277453213.39999998</v>
+        <v>0</v>
       </c>
       <c r="AD4" s="24">
-        <v>276931815.60000002</v>
+        <v>0</v>
       </c>
       <c r="AE4" s="24">
-        <v>275544948.80000001</v>
+        <v>0</v>
       </c>
       <c r="AF4" s="24">
-        <v>274620497.80000001</v>
+        <v>0</v>
       </c>
       <c r="AG4" s="24">
-        <v>273455593.39999998</v>
+        <v>0</v>
       </c>
       <c r="AH4" s="24">
-        <v>271774573.39999998</v>
-      </c>
-    </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>172</v>
       </c>
       <c r="B5" s="24"/>
       <c r="C5" s="24">
-        <v>4956408526.3199997</v>
+        <v>795310233.38999999</v>
       </c>
       <c r="D5" s="24">
-        <v>5057362935.8400002</v>
+        <v>811509478.17999995</v>
       </c>
       <c r="E5" s="24">
-        <v>5258527534.3199997</v>
+        <v>843788549.38999999</v>
       </c>
       <c r="F5" s="24">
-        <v>5429875235.04</v>
+        <v>871283171.58000004</v>
       </c>
       <c r="G5" s="24">
-        <v>5606206123.9200001</v>
+        <v>899577401.09000003</v>
       </c>
       <c r="H5" s="24">
-        <v>5743018119.3599997</v>
+        <v>921530389.72000003</v>
       </c>
       <c r="I5" s="24">
-        <v>5847981880.8000011</v>
+        <v>938372979.10000014</v>
       </c>
       <c r="J5" s="24">
-        <v>5936672121.5999994</v>
+        <v>952604303.19999993</v>
       </c>
       <c r="K5" s="24">
-        <v>6021972305.04</v>
+        <v>966291655.33000004</v>
       </c>
       <c r="L5" s="24">
-        <v>6116383096.3199997</v>
+        <v>981440904.63999987</v>
       </c>
       <c r="M5" s="24">
-        <v>6208602465.6000004</v>
+        <v>996238516.19999993</v>
       </c>
       <c r="N5" s="24">
-        <v>6313991020.5600004</v>
+        <v>1013149268.37</v>
       </c>
       <c r="O5" s="24">
-        <v>6403322912.8800001</v>
+        <v>1027483552.51</v>
       </c>
       <c r="P5" s="24">
-        <v>6488143910.6400003</v>
+        <v>1041094014.03</v>
       </c>
       <c r="Q5" s="24">
-        <v>6574225516.0799999</v>
+        <v>1054906753.91</v>
       </c>
       <c r="R5" s="24">
-        <v>6664113016.0799999</v>
+        <v>1069330191.41</v>
       </c>
       <c r="S5" s="24">
-        <v>6758101089.3599997</v>
+        <v>1084411610.97</v>
       </c>
       <c r="T5" s="24">
-        <v>6839631857.7600002</v>
+        <v>1097494119.02</v>
       </c>
       <c r="U5" s="24">
-        <v>6919997041.1999998</v>
+        <v>1110389596.1500001</v>
       </c>
       <c r="V5" s="24">
-        <v>7002313360.0799999</v>
+        <v>1123598154.4100001</v>
       </c>
       <c r="W5" s="24">
-        <v>7089736112.3999996</v>
+        <v>1137626096.05</v>
       </c>
       <c r="X5" s="24">
-        <v>7179841857.8400002</v>
+        <v>1152084553.4300001</v>
       </c>
       <c r="Y5" s="24">
-        <v>7264295217.8400002</v>
+        <v>1165636023.4300001</v>
       </c>
       <c r="Z5" s="24">
-        <v>7368878245.4400005</v>
+        <v>1182417519.8800001</v>
       </c>
       <c r="AA5" s="24">
-        <v>7456955745.3599997</v>
+        <v>1196550522.97</v>
       </c>
       <c r="AB5" s="24">
-        <v>7554799965.6000004</v>
+        <v>1212250703.7</v>
       </c>
       <c r="AC5" s="24">
-        <v>7653573635.2799997</v>
+        <v>1228100024.8099999</v>
       </c>
       <c r="AD5" s="24">
-        <v>7766317866.96</v>
+        <v>1246191076.1700001</v>
       </c>
       <c r="AE5" s="24">
-        <v>7863371720.1599998</v>
+        <v>1261764433.8199999</v>
       </c>
       <c r="AF5" s="24">
-        <v>7960636938</v>
+        <v>1277371707.25</v>
       </c>
       <c r="AG5" s="24">
-        <v>8075618027.5200005</v>
+        <v>1295821687.04</v>
       </c>
       <c r="AH5" s="24">
-        <v>8157687878.3999996</v>
-      </c>
-    </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.45">
+        <v>1308990696.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>173</v>
       </c>
@@ -7614,345 +7626,345 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>174</v>
       </c>
       <c r="B7" s="24"/>
       <c r="C7" s="24">
         <f>'water &amp; waste'!E22*10^9</f>
-        <v>4517513364.4586792</v>
+        <v>2474460817.2479777</v>
       </c>
       <c r="D7" s="24">
         <f>'water &amp; waste'!F22*10^9</f>
-        <v>4548167224.5369329</v>
+        <v>2509986681.4378862</v>
       </c>
       <c r="E7" s="24">
         <f>'water &amp; waste'!G22*10^9</f>
-        <v>4578821084.6151867</v>
+        <v>2545512545.6277947</v>
       </c>
       <c r="F7" s="24">
         <f>'water &amp; waste'!H22*10^9</f>
-        <v>4609475744.4080324</v>
+        <v>2581037611.9319272</v>
       </c>
       <c r="G7" s="24">
         <f>'water &amp; waste'!I22*10^9</f>
-        <v>4640129604.4862862</v>
+        <v>2616563476.1218357</v>
       </c>
       <c r="H7" s="24">
         <f>'water &amp; waste'!J22*10^9</f>
-        <v>4670783464.5645399</v>
+        <v>2652088542.4259682</v>
       </c>
       <c r="I7" s="24">
         <f>'water &amp; waste'!K22*10^9</f>
-        <v>4701437324.6427927</v>
+        <v>2687614406.6158767</v>
       </c>
       <c r="J7" s="24">
         <f>'water &amp; waste'!L22*10^9</f>
-        <v>4732091984.4356403</v>
+        <v>2723140270.8057852</v>
       </c>
       <c r="K7" s="24">
         <f>'water &amp; waste'!M22*10^9</f>
-        <v>4762745844.5138922</v>
+        <v>2758665337.1099176</v>
       </c>
       <c r="L7" s="24">
         <f>'water &amp; waste'!N22*10^9</f>
-        <v>4793399704.5921459</v>
+        <v>2794191201.2998261</v>
       </c>
       <c r="M7" s="24">
         <f>'water &amp; waste'!O22*10^9</f>
-        <v>4824054364.3849926</v>
+        <v>2829716267.6039586</v>
       </c>
       <c r="N7" s="24">
         <f>'water &amp; waste'!P22*10^9</f>
-        <v>4854708224.4632463</v>
+        <v>2865242131.7938666</v>
       </c>
       <c r="O7" s="24">
         <f>'water &amp; waste'!Q22*10^9</f>
-        <v>4885362084.541501</v>
+        <v>2900767995.9837756</v>
       </c>
       <c r="P7" s="24">
         <f>'water &amp; waste'!R22*10^9</f>
-        <v>4916016744.3343458</v>
+        <v>2936293062.2879076</v>
       </c>
       <c r="Q7" s="24">
         <f>'water &amp; waste'!S22*10^9</f>
-        <v>4946670604.4125996</v>
+        <v>2971818926.4778161</v>
       </c>
       <c r="R7" s="24">
         <f>'water &amp; waste'!T22*10^9</f>
-        <v>4977324464.4908524</v>
+        <v>3007343992.7819486</v>
       </c>
       <c r="S7" s="24">
         <f>'water &amp; waste'!U22*10^9</f>
-        <v>5007979124.2837</v>
+        <v>3042869856.9718575</v>
       </c>
       <c r="T7" s="24">
         <f>'water &amp; waste'!V22*10^9</f>
-        <v>5038632984.3619528</v>
+        <v>3078395721.1617665</v>
       </c>
       <c r="U7" s="24">
         <f>'water &amp; waste'!W22*10^9</f>
-        <v>5069286844.4402056</v>
+        <v>3113920787.465898</v>
       </c>
       <c r="V7" s="24">
         <f>'water &amp; waste'!X22*10^9</f>
-        <v>5099940704.5184593</v>
+        <v>3149446651.6558065</v>
       </c>
       <c r="W7" s="24">
         <f>'water &amp; waste'!Y22*10^9</f>
-        <v>5130595364.311306</v>
+        <v>3184971717.959939</v>
       </c>
       <c r="X7" s="24">
         <f>'water &amp; waste'!Z22*10^9</f>
-        <v>5161249224.3895588</v>
+        <v>3220497582.149848</v>
       </c>
       <c r="Y7" s="24">
         <f>'water &amp; waste'!AA22*10^9</f>
-        <v>5191903084.4678125</v>
+        <v>3256023446.339756</v>
       </c>
       <c r="Z7" s="24">
         <f>'water &amp; waste'!AB22*10^9</f>
-        <v>5222557744.2606592</v>
+        <v>3291548512.6438885</v>
       </c>
       <c r="AA7" s="24">
         <f>'water &amp; waste'!AC22*10^9</f>
-        <v>5253211604.338912</v>
+        <v>3327074376.833797</v>
       </c>
       <c r="AB7" s="24">
         <f>'water &amp; waste'!AD22*10^9</f>
-        <v>5283865464.4171667</v>
+        <v>3362599443.1379294</v>
       </c>
       <c r="AC7" s="24">
         <f>'water &amp; waste'!AE22*10^9</f>
-        <v>5314519324.4954195</v>
+        <v>3398125307.3278379</v>
       </c>
       <c r="AD7" s="24">
         <f>'water &amp; waste'!AF22*10^9</f>
-        <v>5345173984.2882662</v>
+        <v>3433651171.517746</v>
       </c>
       <c r="AE7" s="24">
         <f>'water &amp; waste'!AG22*10^9</f>
-        <v>5375827844.366519</v>
+        <v>3469176237.8218789</v>
       </c>
       <c r="AF7" s="24">
         <f>'water &amp; waste'!AH22*10^9</f>
-        <v>5406481704.4447718</v>
+        <v>3504702102.0117874</v>
       </c>
       <c r="AG7" s="24">
         <f>'water &amp; waste'!AI22*10^9</f>
-        <v>5437136364.2376184</v>
+        <v>3540227168.3159194</v>
       </c>
       <c r="AH7" s="24">
         <f>'water &amp; waste'!AJ22*10^9</f>
-        <v>5467790224.3158731</v>
-      </c>
-    </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.45">
+        <v>3575753032.5058279</v>
+      </c>
+    </row>
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>175</v>
       </c>
       <c r="B8" s="24"/>
       <c r="C8" s="24">
-        <v>8374427606.1599998</v>
+        <v>1129019924.6400001</v>
       </c>
       <c r="D8" s="24">
-        <v>8477032691.8200016</v>
+        <v>1142852892.28</v>
       </c>
       <c r="E8" s="24">
-        <v>8624488199.25</v>
+        <v>1162732484.5</v>
       </c>
       <c r="F8" s="24">
-        <v>8784957500.5499992</v>
+        <v>1184366564.7</v>
       </c>
       <c r="G8" s="24">
-        <v>8910866175.75</v>
+        <v>1201341265.5</v>
       </c>
       <c r="H8" s="24">
-        <v>9049293179.8500004</v>
+        <v>1220003656.9000001</v>
       </c>
       <c r="I8" s="24">
-        <v>9190081925.6399994</v>
+        <v>1238984452.5599999</v>
       </c>
       <c r="J8" s="24">
-        <v>9322366221.6300011</v>
+        <v>1256818699.02</v>
       </c>
       <c r="K8" s="24">
-        <v>9452679604.8299999</v>
+        <v>1274387231.8199999</v>
       </c>
       <c r="L8" s="24">
-        <v>9584798093.6399994</v>
+        <v>1292199124.5599999</v>
       </c>
       <c r="M8" s="24">
-        <v>9720477459</v>
+        <v>1310491086</v>
       </c>
       <c r="N8" s="24">
-        <v>9864671154.0300007</v>
+        <v>1329930928.6199999</v>
       </c>
       <c r="O8" s="24">
-        <v>10024280809.620001</v>
+        <v>1351449113.48</v>
       </c>
       <c r="P8" s="24">
-        <v>10179360423.540001</v>
+        <v>1372356569.1600001</v>
       </c>
       <c r="Q8" s="24">
-        <v>10328642769.059999</v>
+        <v>1392482451.24</v>
       </c>
       <c r="R8" s="24">
-        <v>10486537127.219999</v>
+        <v>1413769383.8800001</v>
       </c>
       <c r="S8" s="24">
-        <v>10636598171.43</v>
+        <v>1434000248.22</v>
       </c>
       <c r="T8" s="24">
-        <v>10776239105.940001</v>
+        <v>1452826298.76</v>
       </c>
       <c r="U8" s="24">
-        <v>10909287288.9</v>
+        <v>1470763530.5999999</v>
       </c>
       <c r="V8" s="24">
-        <v>11041378159.35</v>
+        <v>1488571699.9000001</v>
       </c>
       <c r="W8" s="24">
-        <v>11171734959</v>
+        <v>1506146086</v>
       </c>
       <c r="X8" s="24">
-        <v>11310151113.030001</v>
+        <v>1524807014.6199999</v>
       </c>
       <c r="Y8" s="24">
-        <v>11451235931.52</v>
+        <v>1543827726.0799999</v>
       </c>
       <c r="Z8" s="24">
-        <v>11589730057.290001</v>
+        <v>1562499166.6600001</v>
       </c>
       <c r="AA8" s="24">
-        <v>11733863535.24</v>
+        <v>1581930890.96</v>
       </c>
       <c r="AB8" s="24">
-        <v>11881568755.98</v>
+        <v>1601844148.9200001</v>
       </c>
       <c r="AC8" s="24">
-        <v>12033370743.24</v>
+        <v>1622309722.96</v>
       </c>
       <c r="AD8" s="24">
-        <v>12186099465.540001</v>
+        <v>1642900237.1600001</v>
       </c>
       <c r="AE8" s="24">
-        <v>12339494391.84</v>
+        <v>1663580567.3599999</v>
       </c>
       <c r="AF8" s="24">
-        <v>12494486170.32</v>
+        <v>1684476181.28</v>
       </c>
       <c r="AG8" s="24">
-        <v>12651759746.01</v>
+        <v>1705679421.54</v>
       </c>
       <c r="AH8" s="24">
-        <v>12810756526.26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.45">
+        <v>1727114980.04</v>
+      </c>
+    </row>
+    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>176</v>
       </c>
       <c r="B9" s="24"/>
       <c r="C9" s="24">
-        <v>78447891541.919998</v>
+        <v>10466673472.57</v>
       </c>
       <c r="D9" s="24">
-        <v>78210721533.119995</v>
+        <v>10435029779.02</v>
       </c>
       <c r="E9" s="24">
-        <v>78262112017.440002</v>
+        <v>10441886399.49</v>
       </c>
       <c r="F9" s="24">
-        <v>79436426637.119995</v>
+        <v>10598565788.02</v>
       </c>
       <c r="G9" s="24">
-        <v>80358871152</v>
+        <v>10721640167</v>
       </c>
       <c r="H9" s="24">
-        <v>81428016105.119995</v>
+        <v>10864287609.77</v>
       </c>
       <c r="I9" s="24">
-        <v>82421683532.639999</v>
+        <v>10996864691.190001</v>
       </c>
       <c r="J9" s="24">
-        <v>83535092469.119995</v>
+        <v>11145417922.52</v>
       </c>
       <c r="K9" s="24">
-        <v>84939160114.080002</v>
+        <v>11332751415.93</v>
       </c>
       <c r="L9" s="24">
-        <v>86476138261.919998</v>
+        <v>11537818092.57</v>
       </c>
       <c r="M9" s="24">
-        <v>88076907539.520004</v>
+        <v>11751395908.42</v>
       </c>
       <c r="N9" s="24">
-        <v>89710021495.199997</v>
+        <v>11969289215.450001</v>
       </c>
       <c r="O9" s="24">
-        <v>91304286048</v>
+        <v>12181999158</v>
       </c>
       <c r="P9" s="24">
-        <v>92982201727.199997</v>
+        <v>12405869999.950001</v>
       </c>
       <c r="Q9" s="24">
-        <v>94796408796</v>
+        <v>12647925109.75</v>
       </c>
       <c r="R9" s="24">
-        <v>96774065523.839996</v>
+        <v>12911787997.639999</v>
       </c>
       <c r="S9" s="24">
-        <v>98684964730.080002</v>
+        <v>13166743964.43</v>
       </c>
       <c r="T9" s="24">
-        <v>100482209566.56</v>
+        <v>13406535939.51</v>
       </c>
       <c r="U9" s="24">
-        <v>102381371278.56</v>
+        <v>13659925866.51</v>
       </c>
       <c r="V9" s="24">
-        <v>104181600058.56</v>
+        <v>13900115965.26</v>
       </c>
       <c r="W9" s="24">
-        <v>105989813003.03999</v>
+        <v>14141371327.09</v>
       </c>
       <c r="X9" s="24">
-        <v>107952689682.24001</v>
+        <v>14403262231.540001</v>
       </c>
       <c r="Y9" s="24">
-        <v>110006207726.39999</v>
+        <v>14677246686.9</v>
       </c>
       <c r="Z9" s="24">
-        <v>111912996229.92</v>
+        <v>14931654195.57</v>
       </c>
       <c r="AA9" s="24">
-        <v>113974182305.28</v>
+        <v>15206661734.879999</v>
       </c>
       <c r="AB9" s="24">
-        <v>116026936806.24001</v>
+        <v>15480544316.790001</v>
       </c>
       <c r="AC9" s="24">
-        <v>118015094627.52</v>
+        <v>15745808281.42</v>
       </c>
       <c r="AD9" s="24">
-        <v>119913775473.12</v>
+        <v>15999134050.27</v>
       </c>
       <c r="AE9" s="24">
-        <v>121839066718.56</v>
+        <v>16256010231.51</v>
       </c>
       <c r="AF9" s="24">
-        <v>123715567812.96001</v>
+        <v>16506376733.91</v>
       </c>
       <c r="AG9" s="24">
-        <v>125720449542.72</v>
+        <v>16773872035.620001</v>
       </c>
       <c r="AH9" s="24">
-        <v>127785265657.44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.45">
+        <v>17049363901.99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B11" s="16"/>
     </row>
   </sheetData>

</xml_diff>